<commit_message>
Finished, submission files added. final tweaks complete
</commit_message>
<xml_diff>
--- a/dissertation documents/recommender system occurrences.xlsx
+++ b/dissertation documents/recommender system occurrences.xlsx
@@ -4,22 +4,47 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="23955" windowHeight="12600"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="23955" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="out" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>year</t>
   </si>
   <si>
     <t>results</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Raw Merge</t>
+  </si>
+  <si>
+    <t>Weave</t>
+  </si>
+  <si>
+    <t>DB Size</t>
+  </si>
+  <si>
+    <t>DB Density</t>
+  </si>
+  <si>
+    <t>User Activity</t>
+  </si>
+  <si>
+    <t>ECoRS</t>
+  </si>
+  <si>
+    <t>RoRS</t>
   </si>
 </sst>
 </file>
@@ -771,11 +796,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="133587712"/>
-        <c:axId val="133590016"/>
+        <c:axId val="122120064"/>
+        <c:axId val="122143104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133587712"/>
+        <c:axId val="122120064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,14 +835,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133590016"/>
+        <c:crossAx val="122143104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133590016"/>
+        <c:axId val="122143104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +879,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133587712"/>
+        <c:crossAx val="122120064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -863,7 +888,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1191,7 +1216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
@@ -1417,4 +1442,440 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8">
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8">
+      <c r="B2">
+        <v>0.68217528124667204</v>
+      </c>
+      <c r="C2">
+        <v>0.66564677536658601</v>
+      </c>
+      <c r="D2">
+        <v>0.66101379778065095</v>
+      </c>
+      <c r="E2">
+        <v>0.42945458826732902</v>
+      </c>
+      <c r="F2">
+        <v>0.66101379778065095</v>
+      </c>
+      <c r="G2">
+        <v>0.73760728692233901</v>
+      </c>
+      <c r="H2">
+        <v>0.66101379778065095</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3">
+        <v>0.50237795118609996</v>
+      </c>
+      <c r="C3">
+        <v>0.53548014953841605</v>
+      </c>
+      <c r="D3">
+        <v>0.60618764240142298</v>
+      </c>
+      <c r="E3">
+        <v>0.46951468154320403</v>
+      </c>
+      <c r="F3">
+        <v>0.60618764240142298</v>
+      </c>
+      <c r="G3">
+        <v>0.55986620375631502</v>
+      </c>
+      <c r="H3">
+        <v>0.60618764240142298</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4">
+        <v>0.44772828071834497</v>
+      </c>
+      <c r="C4">
+        <v>0.52733927234161204</v>
+      </c>
+      <c r="D4">
+        <v>0.70244735823007498</v>
+      </c>
+      <c r="E4">
+        <v>0.43385256273029299</v>
+      </c>
+      <c r="F4">
+        <v>0.733938301423251</v>
+      </c>
+      <c r="G4">
+        <v>0.47776814844656101</v>
+      </c>
+      <c r="H4">
+        <v>0.70244735823007498</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5">
+        <v>0.40070964188035801</v>
+      </c>
+      <c r="C5">
+        <v>0.42249536054175302</v>
+      </c>
+      <c r="D5">
+        <v>0.22772539699918301</v>
+      </c>
+      <c r="E5">
+        <v>0.32719301202119999</v>
+      </c>
+      <c r="F5">
+        <v>0.58304802114604803</v>
+      </c>
+      <c r="G5">
+        <v>0.49281530330879397</v>
+      </c>
+      <c r="H5">
+        <v>0.57945839908157903</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6">
+        <v>0.74560296674256599</v>
+      </c>
+      <c r="C6">
+        <v>0.52674261009782197</v>
+      </c>
+      <c r="D6">
+        <v>0.65267455573005595</v>
+      </c>
+      <c r="E6">
+        <v>0.60576527000120595</v>
+      </c>
+      <c r="F6">
+        <v>0.57256124860563196</v>
+      </c>
+      <c r="G6">
+        <v>0.78914585471562904</v>
+      </c>
+      <c r="H6">
+        <v>0.65536315010800505</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7">
+        <v>0.54097452904496002</v>
+      </c>
+      <c r="C7">
+        <v>0.37605844859440302</v>
+      </c>
+      <c r="D7">
+        <v>0.654845570410439</v>
+      </c>
+      <c r="E7">
+        <v>0.54417532901566801</v>
+      </c>
+      <c r="F7">
+        <v>0.654845570410439</v>
+      </c>
+      <c r="G7">
+        <v>0.65261907706837596</v>
+      </c>
+      <c r="H7">
+        <v>0.654845570410439</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8">
+        <v>0.54839585275656999</v>
+      </c>
+      <c r="C8">
+        <v>0.494966885066354</v>
+      </c>
+      <c r="D8">
+        <v>0.540388302619074</v>
+      </c>
+      <c r="E8">
+        <v>0.45981773358029798</v>
+      </c>
+      <c r="F8">
+        <v>0.540388302619074</v>
+      </c>
+      <c r="G8">
+        <v>0.57423798915422897</v>
+      </c>
+      <c r="H8">
+        <v>0.540388302619074</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9">
+        <v>0.53437021670351104</v>
+      </c>
+      <c r="C9">
+        <v>0.46273755749148598</v>
+      </c>
+      <c r="D9">
+        <v>0.58869373840383299</v>
+      </c>
+      <c r="E9">
+        <v>0.54805483655429899</v>
+      </c>
+      <c r="F9">
+        <v>0.58869373840383299</v>
+      </c>
+      <c r="G9">
+        <v>0.59548042422219005</v>
+      </c>
+      <c r="H9">
+        <v>0.58869373840383299</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10">
+        <v>0.54895058816549303</v>
+      </c>
+      <c r="C10">
+        <v>0.49821370324174502</v>
+      </c>
+      <c r="D10">
+        <v>0.77216764461851295</v>
+      </c>
+      <c r="E10">
+        <v>0.120074320200578</v>
+      </c>
+      <c r="F10">
+        <v>0.73311422710902596</v>
+      </c>
+      <c r="G10">
+        <v>0.68119648866187799</v>
+      </c>
+      <c r="H10">
+        <v>0.78417221356257005</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11">
+        <v>0.55489452462768596</v>
+      </c>
+      <c r="C11">
+        <v>0.47686406094623102</v>
+      </c>
+      <c r="D11">
+        <v>0.59852909137921695</v>
+      </c>
+      <c r="E11">
+        <v>0.43963803217799902</v>
+      </c>
+      <c r="F11">
+        <v>0.59852909137921695</v>
+      </c>
+      <c r="G11">
+        <v>0.69730220937471199</v>
+      </c>
+      <c r="H11">
+        <v>0.59852909137921695</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12">
+        <v>0.56594759285733398</v>
+      </c>
+      <c r="C12">
+        <v>0.50907851351868105</v>
+      </c>
+      <c r="D12">
+        <v>0.52662126127752096</v>
+      </c>
+      <c r="E12">
+        <v>0.55508363111912695</v>
+      </c>
+      <c r="F12">
+        <v>0.52662126127752096</v>
+      </c>
+      <c r="G12">
+        <v>0.64363687324385799</v>
+      </c>
+      <c r="H12">
+        <v>0.52662126127752096</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13">
+        <v>0.57091763063215695</v>
+      </c>
+      <c r="C13">
+        <v>0.51657521093320302</v>
+      </c>
+      <c r="D13">
+        <v>0.66722708419071697</v>
+      </c>
+      <c r="E13">
+        <v>0.38039976358362099</v>
+      </c>
+      <c r="F13">
+        <v>0.57922399031712501</v>
+      </c>
+      <c r="G13">
+        <v>0.64928790192563801</v>
+      </c>
+      <c r="H13">
+        <v>0.69763532807619</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14">
+        <v>0.50795602515342497</v>
+      </c>
+      <c r="C14">
+        <v>0.45334804380167898</v>
+      </c>
+      <c r="D14">
+        <v>0.66765159430093102</v>
+      </c>
+      <c r="E14">
+        <v>0.33884847008979102</v>
+      </c>
+      <c r="F14">
+        <v>0.66765159430093102</v>
+      </c>
+      <c r="G14">
+        <v>0.67061865123812303</v>
+      </c>
+      <c r="H14">
+        <v>0.66765159430093102</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15">
+        <v>0.45871356229101001</v>
+      </c>
+      <c r="C15">
+        <v>0.43620197624076301</v>
+      </c>
+      <c r="D15">
+        <v>0.51621307211786205</v>
+      </c>
+      <c r="E15">
+        <v>0.39920820614781999</v>
+      </c>
+      <c r="F15">
+        <v>0.51418022974022703</v>
+      </c>
+      <c r="G15">
+        <v>0.566156630087714</v>
+      </c>
+      <c r="H15">
+        <v>0.55018354940846204</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16">
+        <v>0.66957647160841205</v>
+      </c>
+      <c r="C16">
+        <v>0.49530407880674499</v>
+      </c>
+      <c r="D16">
+        <v>0.63597880421084596</v>
+      </c>
+      <c r="E16">
+        <v>0.66786240533213503</v>
+      </c>
+      <c r="F16">
+        <v>0.63597880421084596</v>
+      </c>
+      <c r="G16">
+        <v>0.66493936342457005</v>
+      </c>
+      <c r="H16">
+        <v>0.63597880421084596</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="B17">
+        <v>0.46663374282521602</v>
+      </c>
+      <c r="C17">
+        <v>0.421386787453773</v>
+      </c>
+      <c r="D17">
+        <v>0.46264437986138601</v>
+      </c>
+      <c r="E17">
+        <v>0.33932316402908502</v>
+      </c>
+      <c r="F17">
+        <v>0.499248495360477</v>
+      </c>
+      <c r="G17">
+        <v>0.49692799809212601</v>
+      </c>
+      <c r="H17">
+        <v>0.57290398691871403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>0.54661999999999999</v>
+      </c>
+      <c r="C18">
+        <v>0.48864999999999997</v>
+      </c>
+      <c r="D18">
+        <v>0.59255999999999998</v>
+      </c>
+      <c r="E18">
+        <v>0.44113999999999998</v>
+      </c>
+      <c r="F18">
+        <v>0.60594999999999999</v>
+      </c>
+      <c r="G18">
+        <v>0.62185000000000001</v>
+      </c>
+      <c r="H18">
+        <v>0.62638000000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>